<commit_message>
fixed add employee scenarios
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/AddEmpData.xlsx
+++ b/src/test/resources/testdata/AddEmpData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thara\IdeaProjects\CucumberFramework_HRMSPortal\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6BE48D-10CE-40FA-B03C-C2A4825697CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B78DCE3-3EC2-4D51-B66B-D3E5743CD2C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="3900" windowWidth="28800" windowHeight="15285" xr2:uid="{F1DBEC02-27F1-4D1B-9102-4360B321DC70}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" xr2:uid="{F1DBEC02-27F1-4D1B-9102-4360B321DC70}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,16 +33,16 @@
     <t>dummy</t>
   </si>
   <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>middleName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
     <t>data</t>
-  </si>
-  <si>
-    <t>firstName</t>
-  </si>
-  <si>
-    <t>middleName</t>
-  </si>
-  <si>
-    <t>lastName</t>
   </si>
 </sst>
 </file>
@@ -397,26 +397,26 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D11:D12"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="14.28515625" customWidth="1"/>
+    <col min="1" max="3" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -424,7 +424,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>